<commit_message>
relaxed identifier cardinality in mspatient
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-nmdp-ethnicity.xlsx
+++ b/docs/StructureDefinition-nmdp-ethnicity.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-07-28T10:15:20-05:00</t>
+    <t>2022-10-31T18:02:56-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -247,53 +247,53 @@
 </t>
   </si>
   <si>
+    <t>Extension.id</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string
+</t>
+  </si>
+  <si>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Extension.extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension
+</t>
+  </si>
+  <si>
+    <t>An Extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
-  </si>
-  <si>
-    <t>Extension.id</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string
-</t>
-  </si>
-  <si>
-    <t>Unique id for inter-element referencing</t>
-  </si>
-  <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>Extension.extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension
-</t>
-  </si>
-  <si>
-    <t>An Extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>Extensions are always sliced by (at least) url</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
   </si>
   <si>
     <t>Extension.url</t>
@@ -1079,7 +1079,7 @@
         <v>76</v>
       </c>
       <c r="AI2" t="s" s="2">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="AJ2" t="s" s="2">
         <v>73</v>
@@ -1087,7 +1087,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
@@ -1098,25 +1098,25 @@
         <v>74</v>
       </c>
       <c r="F3" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="H3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="I3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="J3" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="G3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="H3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="I3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="J3" t="s" s="2">
+      <c r="K3" t="s" s="2">
         <v>80</v>
       </c>
-      <c r="K3" t="s" s="2">
+      <c r="L3" t="s" s="2">
         <v>81</v>
-      </c>
-      <c r="L3" t="s" s="2">
-        <v>82</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1167,27 +1167,27 @@
         <v>73</v>
       </c>
       <c r="AE3" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AF3" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AG3" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AI3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AJ3" t="s" s="2">
         <v>83</v>
-      </c>
-      <c r="AF3" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AG3" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AH3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AI3" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AJ3" t="s" s="2">
-        <v>84</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
@@ -1210,13 +1210,13 @@
         <v>73</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K4" t="s" s="2">
         <v>28</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1255,19 +1255,19 @@
         <v>73</v>
       </c>
       <c r="AA4" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AB4" t="s" s="2">
         <v>88</v>
       </c>
-      <c r="AB4" t="s" s="2">
+      <c r="AC4" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AD4" t="s" s="2">
         <v>89</v>
       </c>
-      <c r="AC4" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AD4" t="s" s="2">
+      <c r="AE4" t="s" s="2">
         <v>90</v>
-      </c>
-      <c r="AE4" t="s" s="2">
-        <v>91</v>
       </c>
       <c r="AF4" t="s" s="2">
         <v>74</v>
@@ -1279,7 +1279,7 @@
         <v>73</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="AJ4" t="s" s="2">
         <v>73</v>
@@ -1295,10 +1295,10 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G5" t="s" s="2">
         <v>73</v>
@@ -1372,10 +1372,10 @@
         <v>92</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AH5" t="s" s="2">
         <v>73</v>
@@ -1400,7 +1400,7 @@
         <v>74</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G6" t="s" s="2">
         <v>73</v>
@@ -1473,7 +1473,7 @@
         <v>74</v>
       </c>
       <c r="AG6" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AH6" t="s" s="2">
         <v>73</v>
@@ -1500,7 +1500,7 @@
         <v>74</v>
       </c>
       <c r="F7" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G7" t="s" s="2">
         <v>73</v>
@@ -1575,7 +1575,7 @@
         <v>74</v>
       </c>
       <c r="AG7" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AH7" t="s" s="2">
         <v>73</v>
@@ -1600,25 +1600,25 @@
         <v>74</v>
       </c>
       <c r="F8" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G8" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="H8" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="I8" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="J8" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="G8" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="H8" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="I8" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="J8" t="s" s="2">
+      <c r="K8" t="s" s="2">
         <v>80</v>
       </c>
-      <c r="K8" t="s" s="2">
+      <c r="L8" t="s" s="2">
         <v>81</v>
-      </c>
-      <c r="L8" t="s" s="2">
-        <v>82</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1669,22 +1669,22 @@
         <v>73</v>
       </c>
       <c r="AE8" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AF8" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AG8" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH8" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AI8" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AJ8" t="s" s="2">
         <v>83</v>
-      </c>
-      <c r="AF8" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AG8" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AH8" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AI8" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AJ8" t="s" s="2">
-        <v>84</v>
       </c>
     </row>
     <row r="9">
@@ -1712,7 +1712,7 @@
         <v>73</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K9" t="s" s="2">
         <v>109</v>
@@ -1759,19 +1759,19 @@
         <v>73</v>
       </c>
       <c r="AA9" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AB9" t="s" s="2">
         <v>88</v>
       </c>
-      <c r="AB9" t="s" s="2">
+      <c r="AC9" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AD9" t="s" s="2">
         <v>89</v>
       </c>
-      <c r="AC9" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AD9" t="s" s="2">
+      <c r="AE9" t="s" s="2">
         <v>90</v>
-      </c>
-      <c r="AE9" t="s" s="2">
-        <v>91</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>74</v>
@@ -1783,10 +1783,10 @@
         <v>73</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10">
@@ -1906,25 +1906,25 @@
         <v>74</v>
       </c>
       <c r="F11" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G11" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="H11" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="I11" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="J11" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="G11" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="H11" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="I11" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="J11" t="s" s="2">
+      <c r="K11" t="s" s="2">
         <v>80</v>
       </c>
-      <c r="K11" t="s" s="2">
+      <c r="L11" t="s" s="2">
         <v>81</v>
-      </c>
-      <c r="L11" t="s" s="2">
-        <v>82</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1975,22 +1975,22 @@
         <v>73</v>
       </c>
       <c r="AE11" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AF11" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AG11" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH11" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AI11" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AJ11" t="s" s="2">
         <v>83</v>
-      </c>
-      <c r="AF11" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AG11" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AH11" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AI11" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AJ11" t="s" s="2">
-        <v>84</v>
       </c>
     </row>
     <row r="12">
@@ -2018,7 +2018,7 @@
         <v>73</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K12" t="s" s="2">
         <v>109</v>
@@ -2065,19 +2065,19 @@
         <v>73</v>
       </c>
       <c r="AA12" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AB12" t="s" s="2">
         <v>88</v>
       </c>
-      <c r="AB12" t="s" s="2">
+      <c r="AC12" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="AD12" t="s" s="2">
         <v>89</v>
       </c>
-      <c r="AC12" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AD12" t="s" s="2">
+      <c r="AE12" t="s" s="2">
         <v>90</v>
-      </c>
-      <c r="AE12" t="s" s="2">
-        <v>91</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>74</v>
@@ -2089,10 +2089,10 @@
         <v>73</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13">
@@ -2108,7 +2108,7 @@
         <v>74</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G13" t="s" s="2">
         <v>73</v>
@@ -2187,7 +2187,7 @@
         <v>74</v>
       </c>
       <c r="AG13" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AH13" t="s" s="2">
         <v>73</v>
@@ -2212,7 +2212,7 @@
         <v>74</v>
       </c>
       <c r="F14" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G14" t="s" s="2">
         <v>73</v>
@@ -2224,7 +2224,7 @@
         <v>113</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K14" t="s" s="2">
         <v>131</v>
@@ -2289,7 +2289,7 @@
         <v>74</v>
       </c>
       <c r="AG14" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AH14" t="s" s="2">
         <v>73</v>
@@ -2314,7 +2314,7 @@
         <v>74</v>
       </c>
       <c r="F15" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G15" t="s" s="2">
         <v>73</v>
@@ -2389,7 +2389,7 @@
         <v>74</v>
       </c>
       <c r="AG15" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AH15" t="s" s="2">
         <v>73</v>
@@ -2414,7 +2414,7 @@
         <v>74</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G16" t="s" s="2">
         <v>73</v>
@@ -2426,7 +2426,7 @@
         <v>113</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K16" t="s" s="2">
         <v>146</v>
@@ -2491,7 +2491,7 @@
         <v>74</v>
       </c>
       <c r="AG16" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AH16" t="s" s="2">
         <v>73</v>
@@ -2516,7 +2516,7 @@
         <v>74</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>73</v>
@@ -2595,7 +2595,7 @@
         <v>74</v>
       </c>
       <c r="AG17" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AH17" t="s" s="2">
         <v>73</v>
@@ -2620,7 +2620,7 @@
         <v>74</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G18" t="s" s="2">
         <v>73</v>
@@ -2632,7 +2632,7 @@
         <v>113</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K18" t="s" s="2">
         <v>160</v>
@@ -2699,7 +2699,7 @@
         <v>74</v>
       </c>
       <c r="AG18" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AH18" t="s" s="2">
         <v>73</v>

</xml_diff>